<commit_message>
Done week 4 timesheet
</commit_message>
<xml_diff>
--- a/Week4/timesheet_Wei_Liu_317932.xlsx
+++ b/Week4/timesheet_Wei_Liu_317932.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="71">
   <si>
     <t>WEEK</t>
   </si>
@@ -248,6 +248,15 @@
   </si>
   <si>
     <t xml:space="preserve">reviewed what is  Dependency Injection(DI), learn on tutorial </t>
+  </si>
+  <si>
+    <t>19/8/2020</t>
+  </si>
+  <si>
+    <t>watched angular tutorial.</t>
+  </si>
+  <si>
+    <t>Share the thoughts of what we have learned.</t>
   </si>
 </sst>
 </file>
@@ -1266,7 +1275,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1326,6 +1335,12 @@
       <c r="B4" t="s">
         <v>60</v>
       </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -1445,6 +1460,12 @@
       </c>
       <c r="B13" t="s">
         <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>